<commit_message>
demo excel file updated
</commit_message>
<xml_diff>
--- a/public/download/demo.xlsx
+++ b/public/download/demo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Ram</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>d@gmail.com42</t>
+  </si>
+  <si>
+    <t>98********</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,8 +429,8 @@
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>34456</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,8 +440,8 @@
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>51521</v>
+      <c r="C3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -448,8 +451,8 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
-        <v>15151</v>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,8 +462,8 @@
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>15615</v>
+      <c r="C5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>